<commit_message>
Why the fit function does not work?
</commit_message>
<xml_diff>
--- a/results/full_sample.xlsx
+++ b/results/full_sample.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20373"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yzho0040\Nonlinear Models in Time Series Analysis\results\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3436CDC4-795D-435A-8D1D-568AC0DDBBAF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -97,8 +91,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -115,18 +109,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -156,29 +144,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -225,7 +201,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -257,27 +233,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -309,24 +267,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -502,42 +442,37 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O23" sqref="J20:O23"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2" t="s">
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+    </row>
+    <row r="2" spans="1:16">
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
@@ -584,7 +519,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -592,24 +527,24 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:16">
+      <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C4">
-        <v>0.70983812144202418</v>
+        <v>0.7098381214420242</v>
       </c>
       <c r="D4">
-        <v>-0.70436485478853184</v>
+        <v>-0.7043648547885318</v>
       </c>
       <c r="E4">
-        <v>2.251668933999882E-2</v>
+        <v>0.02251668933999882</v>
       </c>
       <c r="F4">
-        <v>-0.10484813490714159</v>
+        <v>-0.1048481349071416</v>
       </c>
       <c r="G4">
         <v>-15.68933939555135</v>
@@ -621,61 +556,61 @@
         <v>1.002846617733262</v>
       </c>
       <c r="L4">
-        <v>8.3864230828009894E-4</v>
+        <v>0.0008386423082800989</v>
       </c>
       <c r="M4">
-        <v>-7.3963850497266129E-2</v>
+        <v>-0.07396385049726613</v>
       </c>
       <c r="N4">
-        <v>-2.3461851893578169E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
+        <v>-0.02346185189357817</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
+      <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C5">
-        <v>0.49511579139656953</v>
+        <v>0.4951157913965695</v>
       </c>
       <c r="D5">
-        <v>-0.86882700022037496</v>
+        <v>-0.868827000220375</v>
       </c>
       <c r="E5">
-        <v>7.9208859782597257E-2</v>
+        <v>0.07920885978259726</v>
       </c>
       <c r="F5">
-        <v>5.452386691006994E-2</v>
+        <v>0.05452386691006994</v>
       </c>
       <c r="G5">
-        <v>-50.222284052384239</v>
+        <v>-50.22228405238424</v>
       </c>
       <c r="J5">
-        <v>-0.78640100030164084</v>
+        <v>-0.7864010003016408</v>
       </c>
       <c r="K5">
-        <v>0.69031491996576999</v>
+        <v>0.69031491996577</v>
       </c>
       <c r="L5">
-        <v>6.6833299829989298E-2</v>
+        <v>0.0668332998299893</v>
       </c>
       <c r="M5">
         <v>-0.2478746759656949</v>
       </c>
       <c r="N5">
-        <v>3.686075776349947E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
+        <v>0.003686075776349947</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
+      <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C6">
-        <v>0.71543671845566226</v>
+        <v>0.7154367184556623</v>
       </c>
       <c r="D6">
-        <v>-0.69867754537115934</v>
+        <v>-0.6986775453711593</v>
       </c>
       <c r="E6">
         <v>-0.2216961732569897</v>
@@ -684,62 +619,62 @@
         <v>-0.7903494778953134</v>
       </c>
       <c r="G6">
-        <v>-2.5653276114284971</v>
+        <v>-2.565327611428497</v>
       </c>
       <c r="J6">
-        <v>-2.6355555741313388E-2</v>
+        <v>-0.02635555574131339</v>
       </c>
       <c r="K6">
-        <v>-9.0033631050547372E-5</v>
+        <v>-9.003363105054737E-05</v>
       </c>
       <c r="L6">
-        <v>5.9005999383770331E-2</v>
+        <v>0.05900599938377033</v>
       </c>
       <c r="M6">
         <v>-0.2240063878434384</v>
       </c>
       <c r="N6">
-        <v>-8.3221129544703731E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
+        <v>-0.08322112954470373</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
+      <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C7">
-        <v>0.57413744566493574</v>
+        <v>0.5741374456649357</v>
       </c>
       <c r="D7">
-        <v>-0.81875894247387027</v>
+        <v>-0.8187589424738703</v>
       </c>
       <c r="E7">
-        <v>7.9261925350605208E-2</v>
+        <v>0.07926192535060521</v>
       </c>
       <c r="F7">
-        <v>-7.4912989823483156E-2</v>
+        <v>-0.07491298982348316</v>
       </c>
       <c r="G7">
-        <v>2.2508667372892852E-2</v>
+        <v>0.02250866737289285</v>
       </c>
       <c r="J7">
-        <v>0.25872214390613613</v>
+        <v>0.2587221439061361</v>
       </c>
       <c r="K7">
         <v>-0.4714694013678129</v>
       </c>
       <c r="L7">
-        <v>7.6593378076260474E-2</v>
+        <v>0.07659337807626047</v>
       </c>
       <c r="M7">
-        <v>-8.9746822573369064E-2</v>
+        <v>-0.08974682257336906</v>
       </c>
       <c r="N7">
-        <v>2.3478174772059251E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+        <v>0.02347817477205925</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
+      <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -749,159 +684,159 @@
         <v>-0.7044579395342766</v>
       </c>
       <c r="D8">
-        <v>0.70974574297510817</v>
+        <v>0.7097457429751082</v>
       </c>
       <c r="E8">
-        <v>0.12625280270313069</v>
+        <v>0.1262528027031307</v>
       </c>
       <c r="F8">
-        <v>-0.24308974415067439</v>
+        <v>-0.2430897441506744</v>
       </c>
       <c r="G8">
-        <v>7.8509181153839176</v>
+        <v>7.850918115383918</v>
       </c>
       <c r="J8">
-        <v>43.191122428336563</v>
+        <v>43.19112242833656</v>
       </c>
       <c r="K8">
-        <v>40.112354687576193</v>
+        <v>40.11235468757619</v>
       </c>
       <c r="L8">
-        <v>-0.37237354859387872</v>
+        <v>-0.3723735485938787</v>
       </c>
       <c r="M8">
-        <v>0.26427200024478392</v>
+        <v>0.2642720002447839</v>
       </c>
       <c r="N8">
-        <v>-10.953036997058859</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
+        <v>-10.95303699705886</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
+      <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C9">
-        <v>-0.49505846620801658</v>
+        <v>-0.4950584662080166</v>
       </c>
       <c r="D9">
         <v>0.8688597570740404</v>
       </c>
       <c r="E9">
-        <v>7.9204411905135885E-2</v>
+        <v>0.07920441190513589</v>
       </c>
       <c r="F9">
-        <v>5.4409534199996737E-2</v>
+        <v>0.05440953419999674</v>
       </c>
       <c r="G9">
-        <v>45.509892315108331</v>
+        <v>45.50989231510833</v>
       </c>
       <c r="J9">
-        <v>0.78977958327006703</v>
+        <v>0.789779583270067</v>
       </c>
       <c r="K9">
-        <v>-0.69352173618697222</v>
+        <v>-0.6935217361869722</v>
       </c>
       <c r="L9">
-        <v>6.669109430122834E-2</v>
+        <v>0.06669109430122834</v>
       </c>
       <c r="M9">
-        <v>-0.24909759312748991</v>
+        <v>-0.2490975931274899</v>
       </c>
       <c r="N9">
         <v>1.567155538521835</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
+    <row r="10" spans="1:16">
+      <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C10">
-        <v>-0.67846261301456334</v>
+        <v>-0.6784626130145633</v>
       </c>
       <c r="D10">
-        <v>0.73463495729367922</v>
+        <v>0.7346349572936792</v>
       </c>
       <c r="E10">
-        <v>0.32250596758347011</v>
+        <v>0.3225059675834701</v>
       </c>
       <c r="F10">
-        <v>0.32552856466992341</v>
+        <v>0.3255285646699234</v>
       </c>
       <c r="G10">
         <v>1.202325691000929</v>
       </c>
       <c r="J10">
-        <v>5.4811746545564217</v>
+        <v>5.481174654556422</v>
       </c>
       <c r="K10">
-        <v>3.2366818586812389</v>
+        <v>3.236681858681239</v>
       </c>
       <c r="L10">
         <v>-1.072841594960227</v>
       </c>
       <c r="M10">
-        <v>0.60035413900127699</v>
+        <v>0.600354139001277</v>
       </c>
       <c r="N10">
         <v>-1.294523408058434</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
+    <row r="11" spans="1:16">
+      <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C11">
-        <v>0.76158097341382347</v>
+        <v>0.7615809734138235</v>
       </c>
       <c r="D11">
         <v>-0.6480697665353834</v>
       </c>
       <c r="E11">
-        <v>6.775331007101229E-2</v>
+        <v>0.06775331007101229</v>
       </c>
       <c r="F11">
-        <v>-0.13757963951778129</v>
+        <v>-0.1375796395177813</v>
       </c>
       <c r="G11">
-        <v>1.5439112265103161</v>
+        <v>1.543911226510316</v>
       </c>
       <c r="J11">
-        <v>-0.25377345471835522</v>
+        <v>-0.2537734547183552</v>
       </c>
       <c r="K11">
-        <v>0.46635039353334617</v>
+        <v>0.4663503935333462</v>
       </c>
       <c r="L11">
-        <v>7.652194954252714E-2</v>
+        <v>0.07652194954252714</v>
       </c>
       <c r="M11">
-        <v>-9.0178318985540393E-2</v>
+        <v>-0.09017831898554039</v>
       </c>
       <c r="N11">
         <v>1.547280156065749</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+    <row r="12" spans="1:16">
+      <c r="A12" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C12">
-        <v>0.97748599018530968</v>
+        <v>0.9774859901853097</v>
       </c>
       <c r="D12">
-        <v>0.21100035759992181</v>
+        <v>0.2110003575999218</v>
       </c>
       <c r="E12">
-        <v>-0.75045994969752727</v>
+        <v>-0.7504599496975273</v>
       </c>
       <c r="F12">
-        <v>0.79978819068771179</v>
+        <v>0.7997881906877118</v>
       </c>
       <c r="G12">
         <v>2.079635739742439</v>
@@ -910,26 +845,26 @@
         <v>-24.43232322829261</v>
       </c>
       <c r="J12">
-        <v>-0.88783677203780675</v>
+        <v>-0.8878367720378068</v>
       </c>
       <c r="K12">
-        <v>0.88289425337602601</v>
+        <v>0.882894253376026</v>
       </c>
       <c r="L12">
-        <v>8.2064264308178412E-4</v>
+        <v>0.0008206426430817841</v>
       </c>
       <c r="M12">
-        <v>-7.599528089600012E-2</v>
+        <v>-0.07599528089600012</v>
       </c>
       <c r="N12">
-        <v>-2.3565256314074461E-2</v>
+        <v>-0.02356525631407446</v>
       </c>
       <c r="O12">
         <v>1.136082901697407</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
+    <row r="13" spans="1:16">
+      <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
         <v>21</v>
       </c>
@@ -937,169 +872,169 @@
         <v>0.7516053734108572</v>
       </c>
       <c r="D13">
-        <v>-0.65961327437878847</v>
+        <v>-0.6596132743787885</v>
       </c>
       <c r="E13">
-        <v>6.6742912662351966E-2</v>
+        <v>0.06674291266235197</v>
       </c>
       <c r="F13">
         <v>-0.2482506625175557</v>
       </c>
       <c r="G13">
-        <v>3.685920950879629E-3</v>
+        <v>0.003685920950879629</v>
       </c>
       <c r="H13">
-        <v>-1.0478324228856419</v>
+        <v>-1.047832422885642</v>
       </c>
       <c r="J13">
-        <v>2.8757908510845082E-4</v>
+        <v>0.0002875790851084508</v>
       </c>
       <c r="K13">
-        <v>7.0179709333359637E-4</v>
+        <v>0.0007017970933335964</v>
       </c>
       <c r="L13">
-        <v>7.8532202946758903E-2</v>
+        <v>0.0785322029467589</v>
       </c>
       <c r="M13">
         <v>-0.1616280178121785</v>
       </c>
       <c r="N13">
-        <v>1.125200711491281E-2</v>
+        <v>0.01125200711491281</v>
       </c>
       <c r="O13">
-        <v>-2.1486715751460931E-4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
+        <v>-0.0002148671575146093</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
+      <c r="A14" s="1"/>
       <c r="B14" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C14">
-        <v>0.98809428606397542</v>
+        <v>0.9880942860639754</v>
       </c>
       <c r="D14">
-        <v>0.15384954602904269</v>
+        <v>0.1538495460290427</v>
       </c>
       <c r="E14">
-        <v>6.0807732241074518E-2</v>
+        <v>0.06080773224107452</v>
       </c>
       <c r="F14">
-        <v>-0.22034787435611389</v>
+        <v>-0.2203478743561139</v>
       </c>
       <c r="G14">
-        <v>3.2239462855504701</v>
+        <v>3.22394628555047</v>
       </c>
       <c r="H14">
-        <v>2.3583470097455862E-2</v>
+        <v>0.02358347009745586</v>
       </c>
       <c r="J14">
-        <v>3.2600966091757042E-2</v>
+        <v>0.03260096609175704</v>
       </c>
       <c r="K14">
-        <v>2.3985705457761589E-5</v>
+        <v>2.398570545776159E-05</v>
       </c>
       <c r="L14">
-        <v>5.9209391370278121E-2</v>
+        <v>0.05920939137027812</v>
       </c>
       <c r="M14">
         <v>-0.223982863030423</v>
       </c>
       <c r="N14">
-        <v>-8.3093316360210431E-2</v>
+        <v>-0.08309331636021043</v>
       </c>
       <c r="O14">
-        <v>-0.80894222523960846</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
+        <v>-0.8089422252396085</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16">
+      <c r="A15" s="1"/>
       <c r="B15" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C15">
-        <v>0.70330509532080376</v>
+        <v>0.7033050953208038</v>
       </c>
       <c r="D15">
-        <v>0.71088856446113091</v>
+        <v>0.7108885644611309</v>
       </c>
       <c r="E15">
-        <v>7.3754422813810463E-2</v>
+        <v>0.07375442281381046</v>
       </c>
       <c r="F15">
         <v>-0.1054358592556594</v>
       </c>
       <c r="G15">
-        <v>2.475336491081646E-2</v>
+        <v>0.02475336491081646</v>
       </c>
       <c r="H15">
         <v>-0.1271351954521083</v>
       </c>
       <c r="J15">
-        <v>5.5641414995105166E-4</v>
+        <v>0.0005564141499510517</v>
       </c>
       <c r="K15">
-        <v>5.7838995354618625E-4</v>
+        <v>0.0005783899535461862</v>
       </c>
       <c r="L15">
-        <v>7.8532205641704808E-2</v>
+        <v>0.07853220564170481</v>
       </c>
       <c r="M15">
-        <v>-0.16162851884415499</v>
+        <v>-0.161628518844155</v>
       </c>
       <c r="N15">
-        <v>1.1251999507145231E-2</v>
+        <v>0.01125199950714523</v>
       </c>
       <c r="O15">
-        <v>-1.7354920781541451E-5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+        <v>-1.735492078154145E-05</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16">
+      <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C16">
-        <v>-0.70907181059329516</v>
+        <v>-0.7090718105932952</v>
       </c>
       <c r="D16">
-        <v>0.70513628551340723</v>
+        <v>0.7051362855134072</v>
       </c>
       <c r="E16">
-        <v>8.310745674540872E-4</v>
+        <v>0.0008310745674540872</v>
       </c>
       <c r="F16">
-        <v>-7.6038457165460163E-2</v>
+        <v>-0.07603845716546016</v>
       </c>
       <c r="G16">
-        <v>-1.5942702240422171</v>
+        <v>-1.594270224042217</v>
       </c>
       <c r="H16">
-        <v>1.4226613281597691</v>
+        <v>1.422661328159769</v>
       </c>
       <c r="J16">
-        <v>-380.69353359258099</v>
+        <v>-380.693533592581</v>
       </c>
       <c r="K16">
-        <v>378.61533724790269</v>
+        <v>378.6153372479027</v>
       </c>
       <c r="L16">
-        <v>9.1999764516602692E-4</v>
+        <v>0.0009199976451660269</v>
       </c>
       <c r="M16">
-        <v>-7.5847136801971124E-2</v>
+        <v>-0.07584713680197112</v>
       </c>
       <c r="N16">
         <v>1.593964232857632</v>
       </c>
       <c r="O16">
-        <v>-2.6491757523106501E-3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
+        <v>-0.00264917575231065</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16">
+      <c r="A17" s="1"/>
       <c r="B17" s="1" t="s">
         <v>21</v>
       </c>
@@ -1107,13 +1042,13 @@
         <v>0.7516508672646135</v>
       </c>
       <c r="D17">
-        <v>-0.65956137576566221</v>
+        <v>-0.6595613757656622</v>
       </c>
       <c r="E17">
-        <v>6.6762156834227246E-2</v>
+        <v>0.06676215683422725</v>
       </c>
       <c r="F17">
-        <v>-0.24880239796906251</v>
+        <v>-0.2488023979690625</v>
       </c>
       <c r="G17">
         <v>1.567108760181873</v>
@@ -1128,7 +1063,7 @@
         <v>2.194267637502465</v>
       </c>
       <c r="L17">
-        <v>6.6695103701301828E-2</v>
+        <v>0.06669510370130183</v>
       </c>
       <c r="M17">
         <v>-0.2498806588699114</v>
@@ -1137,40 +1072,40 @@
         <v>1.567050667144039</v>
       </c>
       <c r="O17">
-        <v>-0.31458834648964901</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
+        <v>-0.314588346489649</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16">
+      <c r="A18" s="1"/>
       <c r="B18" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C18">
-        <v>-4.7821474203436458E-2</v>
+        <v>-0.04782147420343646</v>
       </c>
       <c r="D18">
-        <v>-0.99885589943596209</v>
+        <v>-0.9988558994359621</v>
       </c>
       <c r="E18">
-        <v>7.5881792734004971E-2</v>
+        <v>0.07588179273400497</v>
       </c>
       <c r="F18">
-        <v>-0.18973202568177511</v>
+        <v>-0.1897320256817751</v>
       </c>
       <c r="G18">
         <v>-1.613683767079483</v>
       </c>
       <c r="H18">
-        <v>1.7991324870810101E-2</v>
+        <v>0.0179913248708101</v>
       </c>
       <c r="J18">
         <v>1.610638011049659</v>
       </c>
       <c r="K18">
-        <v>3.877913977938663E-3</v>
+        <v>0.003877913977938663</v>
       </c>
       <c r="L18">
-        <v>5.8675334495227077E-2</v>
+        <v>0.05867533449522708</v>
       </c>
       <c r="M18">
         <v>-0.2236385302136577</v>
@@ -1179,40 +1114,40 @@
         <v>1.65419121399958</v>
       </c>
       <c r="O18">
-        <v>1.6408833151314441E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
+        <v>0.01640883315131444</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16">
+      <c r="A19" s="1"/>
       <c r="B19" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C19">
-        <v>0.75784084813153518</v>
+        <v>0.7578408481315352</v>
       </c>
       <c r="D19">
         <v>0.6524395023687195</v>
       </c>
       <c r="E19">
-        <v>7.3887179054872923E-2</v>
+        <v>0.07388717905487292</v>
       </c>
       <c r="F19">
         <v>-0.1070431088417302</v>
       </c>
       <c r="G19">
-        <v>1.5461189536237001</v>
+        <v>1.5461189536237</v>
       </c>
       <c r="H19">
-        <v>0.12636543538126541</v>
+        <v>0.1263654353812654</v>
       </c>
       <c r="J19">
-        <v>0.26942385938835889</v>
+        <v>0.2694238593883589</v>
       </c>
       <c r="K19">
-        <v>0.32324310727701222</v>
+        <v>0.3232431072770122</v>
       </c>
       <c r="L19">
-        <v>7.3541445216137452E-2</v>
+        <v>0.07354144521613745</v>
       </c>
       <c r="M19">
         <v>-0.1055496786318387</v>
@@ -1221,275 +1156,275 @@
         <v>1.546091199902045</v>
       </c>
       <c r="O19">
-        <v>0.30534153998551328</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+        <v>0.3053415399855133</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16">
+      <c r="A20" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C20">
-        <v>0.70704199775784571</v>
+        <v>0.7070419977578457</v>
       </c>
       <c r="D20">
-        <v>0.70717155868049053</v>
+        <v>0.7071715586804905</v>
       </c>
       <c r="E20">
         <v>0.1020627174815323</v>
       </c>
       <c r="F20">
-        <v>-0.18925521843347801</v>
+        <v>-0.189255218433478</v>
       </c>
       <c r="G20">
-        <v>7.0836174693707994</v>
+        <v>7.083617469370799</v>
       </c>
       <c r="H20">
-        <v>4.1887945917852294</v>
-      </c>
-      <c r="J20" s="3">
-        <v>9.971509642475744E-4</v>
-      </c>
-      <c r="K20" s="3">
-        <v>1.001199021049856E-3</v>
-      </c>
-      <c r="L20" s="3">
-        <v>7.8532220980738379E-2</v>
-      </c>
-      <c r="M20" s="3">
-        <v>-0.16162608749840601</v>
-      </c>
-      <c r="N20" s="3">
-        <v>1.1251753636457159E-2</v>
-      </c>
-      <c r="O20" s="3">
-        <v>9.9906501665926548E-4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
+        <v>4.188794591785229</v>
+      </c>
+      <c r="J20">
+        <v>0.0009971509642475744</v>
+      </c>
+      <c r="K20">
+        <v>0.001001199021049856</v>
+      </c>
+      <c r="L20">
+        <v>0.07853222098073838</v>
+      </c>
+      <c r="M20">
+        <v>-0.161626087498406</v>
+      </c>
+      <c r="N20">
+        <v>0.01125175363645716</v>
+      </c>
+      <c r="O20">
+        <v>0.0009990650166592655</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16">
+      <c r="A21" s="1"/>
       <c r="B21" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C21">
-        <v>0.70711095485036612</v>
+        <v>0.7071109548503661</v>
       </c>
       <c r="D21">
-        <v>0.70710260750027509</v>
+        <v>0.7071026075002751</v>
       </c>
       <c r="E21">
-        <v>7.85311220229791E-2</v>
+        <v>0.0785311220229791</v>
       </c>
       <c r="F21">
-        <v>-0.16165760595055631</v>
+        <v>-0.1616576059505563</v>
       </c>
       <c r="G21">
-        <v>1.1254258054091391E-2</v>
+        <v>0.01125425805409139</v>
       </c>
       <c r="H21">
-        <v>1.2103813282985961E-2</v>
-      </c>
-      <c r="J21" s="3">
-        <v>9.9999999999999221E-4</v>
-      </c>
-      <c r="K21" s="3">
-        <v>1.000000000000002E-3</v>
-      </c>
-      <c r="L21" s="3">
-        <v>7.8532213370099205E-2</v>
-      </c>
-      <c r="M21" s="3">
-        <v>-0.16162629761485159</v>
-      </c>
-      <c r="N21" s="3">
-        <v>1.125175290379125E-2</v>
-      </c>
-      <c r="O21" s="3">
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
+        <v>0.01210381328298596</v>
+      </c>
+      <c r="J21">
+        <v>0.0009999999999999922</v>
+      </c>
+      <c r="K21">
+        <v>0.001000000000000002</v>
+      </c>
+      <c r="L21">
+        <v>0.0785322133700992</v>
+      </c>
+      <c r="M21">
+        <v>-0.1616262976148516</v>
+      </c>
+      <c r="N21">
+        <v>0.01125175290379125</v>
+      </c>
+      <c r="O21">
+        <v>0.001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16">
+      <c r="A22" s="1"/>
       <c r="B22" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C22">
-        <v>0.70009363730979834</v>
+        <v>0.7000936373097983</v>
       </c>
       <c r="D22">
-        <v>0.71405104789388296</v>
+        <v>0.714051047893883</v>
       </c>
       <c r="E22">
         <v>0.1021026990491623</v>
       </c>
       <c r="F22">
-        <v>-0.18924597909404661</v>
+        <v>-0.1892459790940466</v>
       </c>
       <c r="G22">
-        <v>4.7257301880481011</v>
+        <v>4.725730188048101</v>
       </c>
       <c r="H22">
         <v>3.478380491093048</v>
       </c>
-      <c r="J22" s="3">
-        <v>9.9581012406938971E-4</v>
-      </c>
-      <c r="K22" s="3">
-        <v>9.9670813416361925E-4</v>
-      </c>
-      <c r="L22" s="3">
-        <v>7.8532214837737438E-2</v>
-      </c>
-      <c r="M22" s="3">
-        <v>-0.16162616476768071</v>
-      </c>
-      <c r="N22" s="3">
-        <v>1.1251753444324591E-2</v>
-      </c>
-      <c r="O22" s="3">
-        <v>9.9621380466184076E-4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
+      <c r="J22">
+        <v>0.0009958101240693897</v>
+      </c>
+      <c r="K22">
+        <v>0.0009967081341636192</v>
+      </c>
+      <c r="L22">
+        <v>0.07853221483773744</v>
+      </c>
+      <c r="M22">
+        <v>-0.1616261647676807</v>
+      </c>
+      <c r="N22">
+        <v>0.01125175344432459</v>
+      </c>
+      <c r="O22">
+        <v>0.0009962138046618408</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16">
+      <c r="A23" s="1"/>
       <c r="B23" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C23">
-        <v>0.70710984093005891</v>
+        <v>0.7071098409300589</v>
       </c>
       <c r="D23">
-        <v>0.70710372142988254</v>
+        <v>0.7071037214298825</v>
       </c>
       <c r="E23">
-        <v>7.8529649639356075E-2</v>
+        <v>0.07852964963935608</v>
       </c>
       <c r="F23">
-        <v>-0.16163639805617569</v>
+        <v>-0.1616363980561757</v>
       </c>
       <c r="G23">
-        <v>1.1256295296992571E-2</v>
+        <v>0.01125629529699257</v>
       </c>
       <c r="H23">
-        <v>1.7258180881767039E-2</v>
-      </c>
-      <c r="J23" s="3">
-        <v>1.000000000000008E-3</v>
-      </c>
-      <c r="K23" s="3">
-        <v>1.0000000000000011E-3</v>
-      </c>
-      <c r="L23" s="3">
-        <v>7.8532219529515931E-2</v>
-      </c>
-      <c r="M23" s="3">
+        <v>0.01725818088176704</v>
+      </c>
+      <c r="J23">
+        <v>0.001000000000000008</v>
+      </c>
+      <c r="K23">
+        <v>0.001000000000000001</v>
+      </c>
+      <c r="L23">
+        <v>0.07853221952951593</v>
+      </c>
+      <c r="M23">
         <v>-0.1616261733660494</v>
       </c>
-      <c r="N23" s="3">
-        <v>1.1251752963368951E-2</v>
-      </c>
-      <c r="O23" s="3">
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
+      <c r="N23">
+        <v>0.01125175296336895</v>
+      </c>
+      <c r="O23">
+        <v>0.001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16">
+      <c r="A24" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C24">
-        <v>0.70518178191075143</v>
+        <v>0.7051817819107514</v>
       </c>
       <c r="D24">
-        <v>0.70902655413036253</v>
+        <v>0.7090265541303625</v>
       </c>
       <c r="E24">
-        <v>-1.9851678873965131</v>
+        <v>-1.985167887396513</v>
       </c>
       <c r="F24">
-        <v>2.2668613227890888</v>
+        <v>2.266861322789089</v>
       </c>
       <c r="G24">
-        <v>-8.0194507528231641E-3</v>
+        <v>-0.008019450752823164</v>
       </c>
       <c r="H24">
-        <v>-8.3429898001653644</v>
+        <v>-8.342989800165364</v>
       </c>
       <c r="J24">
-        <v>-1.4850254036086441E-4</v>
+        <v>-0.0001485025403608644</v>
       </c>
       <c r="K24">
-        <v>1.381400503901313E-5</v>
+        <v>1.381400503901313E-05</v>
       </c>
       <c r="L24">
-        <v>0.10201675887338919</v>
+        <v>0.1020167588733892</v>
       </c>
       <c r="M24">
-        <v>-0.18926002646672671</v>
+        <v>-0.1892600264667267</v>
       </c>
       <c r="N24">
-        <v>7.0767459928296726E-4</v>
+        <v>0.0007076745992829673</v>
       </c>
       <c r="O24">
-        <v>-3.6212406469729848E-4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A25" s="2"/>
+        <v>-0.0003621240646972985</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16">
+      <c r="A25" s="1"/>
       <c r="B25" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C25">
-        <v>-0.73154034127247047</v>
+        <v>-0.7315403412724705</v>
       </c>
       <c r="D25">
-        <v>0.68179815964777923</v>
+        <v>0.6817981596477792</v>
       </c>
       <c r="E25">
-        <v>6.7960067362288393E-2</v>
+        <v>0.06796006736228839</v>
       </c>
       <c r="F25">
-        <v>-0.22529372082457599</v>
+        <v>-0.225293720824576</v>
       </c>
       <c r="G25">
-        <v>-2.0163458111271858E-2</v>
+        <v>-0.02016345811127186</v>
       </c>
       <c r="H25">
-        <v>-12.942195339598189</v>
+        <v>-12.94219533959819</v>
       </c>
       <c r="J25">
-        <v>1.0019716376503071E-3</v>
+        <v>0.001001971637650307</v>
       </c>
       <c r="K25">
-        <v>1.004281574750939E-3</v>
+        <v>0.001004281574750939</v>
       </c>
       <c r="L25">
         <v>0.1020167524572109</v>
       </c>
       <c r="M25">
-        <v>-0.18926191240905291</v>
+        <v>-0.1892619124090529</v>
       </c>
       <c r="N25">
-        <v>9.1907178563095833E-4</v>
+        <v>0.0009190717856309583</v>
       </c>
       <c r="O25">
-        <v>9.6306814523771593E-4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A26" s="2"/>
+        <v>0.0009630681452377159</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16">
+      <c r="A26" s="1"/>
       <c r="B26" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C26">
-        <v>0.70345919058338768</v>
+        <v>0.7034591905833877</v>
       </c>
       <c r="D26">
-        <v>0.71073565211593603</v>
+        <v>0.710735652115936</v>
       </c>
       <c r="E26">
         <v>-1.985168333440249</v>
@@ -1498,43 +1433,43 @@
         <v>2.266870752791478</v>
       </c>
       <c r="G26">
-        <v>-7.4017242328029221E-3</v>
+        <v>-0.007401724232802922</v>
       </c>
       <c r="H26">
-        <v>-7.2964699542887619</v>
+        <v>-7.296469954288762</v>
       </c>
       <c r="J26">
-        <v>-1.6489173404039909E-4</v>
+        <v>-0.0001648917340403991</v>
       </c>
       <c r="K26">
-        <v>7.6051599740764003E-5</v>
+        <v>7.6051599740764E-05</v>
       </c>
       <c r="L26">
         <v>0.10201676623047</v>
       </c>
       <c r="M26">
-        <v>-0.18925991178385401</v>
+        <v>-0.189259911783854</v>
       </c>
       <c r="N26">
-        <v>7.0116407361059711E-4</v>
+        <v>0.0007011640736105971</v>
       </c>
       <c r="O26">
-        <v>-3.2976941328091729E-4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A27" s="2"/>
+        <v>-0.0003297694132809173</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16">
+      <c r="A27" s="1"/>
       <c r="B27" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C27">
-        <v>-0.91822804520661561</v>
+        <v>-0.9182280452066156</v>
       </c>
       <c r="D27">
-        <v>0.39605211871361301</v>
+        <v>0.396052118713613</v>
       </c>
       <c r="E27">
-        <v>7.1971190594253567E-2</v>
+        <v>0.07197119059425357</v>
       </c>
       <c r="F27">
         <v>-0.1086570392507689</v>
@@ -1546,229 +1481,229 @@
         <v>-2.684786587616844</v>
       </c>
       <c r="J27">
-        <v>1.005200338459678E-3</v>
+        <v>0.001005200338459678</v>
       </c>
       <c r="K27">
-        <v>1.0043963142674489E-3</v>
+        <v>0.001004396314267449</v>
       </c>
       <c r="L27">
-        <v>0.10201675093185859</v>
+        <v>0.1020167509318586</v>
       </c>
       <c r="M27">
         <v>-0.1892618018819007</v>
       </c>
       <c r="N27">
-        <v>9.2326789306961476E-4</v>
+        <v>0.0009232678930696148</v>
       </c>
       <c r="O27">
-        <v>9.6685643445508485E-4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
+        <v>0.0009668564344550849</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16">
+      <c r="A28" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C28">
-        <v>-0.17041674339105989</v>
+        <v>-0.1704167433910599</v>
       </c>
       <c r="D28">
-        <v>0.98537207906053081</v>
+        <v>0.9853720790605308</v>
       </c>
       <c r="E28">
-        <v>9.4352443705396166E-2</v>
+        <v>0.09435244370539617</v>
       </c>
       <c r="F28">
-        <v>-9.9866690105085393E-2</v>
+        <v>-0.09986669010508539</v>
       </c>
       <c r="G28">
-        <v>8.9072535308970122E-2</v>
+        <v>0.08907253530897012</v>
       </c>
       <c r="H28">
-        <v>2.3589845805848161E-2</v>
+        <v>0.02358984580584816</v>
       </c>
       <c r="I28">
-        <v>-1.104977870285756E-3</v>
+        <v>-0.001104977870285756</v>
       </c>
       <c r="J28">
-        <v>-0.87918796687619516</v>
+        <v>-0.8791879668761952</v>
       </c>
       <c r="K28">
-        <v>0.87435197504119633</v>
+        <v>0.8743519750411963</v>
       </c>
       <c r="L28">
-        <v>5.4178788664583169E-4</v>
+        <v>0.0005417878866458317</v>
       </c>
       <c r="M28">
-        <v>-7.6459113733225989E-2</v>
+        <v>-0.07645911373322599</v>
       </c>
       <c r="N28">
-        <v>-2.313861396580737E-2</v>
+        <v>-0.02313861396580737</v>
       </c>
       <c r="O28">
         <v>1.141644745624486</v>
       </c>
       <c r="P28">
-        <v>-7.4145764413061175E-4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A29" s="2"/>
+        <v>-0.0007414576441306117</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16">
+      <c r="A29" s="1"/>
       <c r="B29" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C29">
-        <v>0.75314222481158088</v>
+        <v>0.7531422248115809</v>
       </c>
       <c r="D29">
-        <v>-0.65785790282127932</v>
+        <v>-0.6578579028212793</v>
       </c>
       <c r="E29">
-        <v>6.666808365576414E-2</v>
+        <v>0.06666808365576414</v>
       </c>
       <c r="F29">
-        <v>-0.24916960816548181</v>
+        <v>-0.2491696081654818</v>
       </c>
       <c r="G29">
-        <v>4.1239159824263552E-3</v>
+        <v>0.004123915982426355</v>
       </c>
       <c r="H29">
         <v>-1.07555160128354</v>
       </c>
       <c r="I29">
-        <v>-2.6206434129941338</v>
+        <v>-2.620643412994134</v>
       </c>
       <c r="J29">
-        <v>2.872417743139459E-4</v>
+        <v>0.0002872417743139459</v>
       </c>
       <c r="K29">
-        <v>7.0150145073151937E-4</v>
+        <v>0.0007015014507315194</v>
       </c>
       <c r="L29">
-        <v>7.853220761447785E-2</v>
+        <v>0.07853220761447785</v>
       </c>
       <c r="M29">
-        <v>-0.16162788890519891</v>
+        <v>-0.1616278889051989</v>
       </c>
       <c r="N29">
-        <v>1.125177000165874E-2</v>
+        <v>0.01125177000165874</v>
       </c>
       <c r="O29">
-        <v>-2.147523895330708E-4</v>
+        <v>-0.0002147523895330708</v>
       </c>
       <c r="P29">
-        <v>9.997502560562786E-4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A30" s="2"/>
+        <v>0.0009997502560562786</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16">
+      <c r="A30" s="1"/>
       <c r="B30" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C30">
-        <v>-5.3952928951015583E-2</v>
+        <v>-0.05395292895101558</v>
       </c>
       <c r="D30">
-        <v>0.99854348000635695</v>
+        <v>0.998543480006357</v>
       </c>
       <c r="E30">
-        <v>5.1058295613596892E-2</v>
+        <v>0.05105829561359689</v>
       </c>
       <c r="F30">
         <v>-0.1954875763377007</v>
       </c>
       <c r="G30">
-        <v>-0.18774474838716509</v>
+        <v>-0.1877447483871651</v>
       </c>
       <c r="H30">
-        <v>-0.12862202168275999</v>
+        <v>-0.12862202168276</v>
       </c>
       <c r="I30">
-        <v>-1.9665906611802151E-2</v>
+        <v>-0.01966590661180215</v>
       </c>
       <c r="J30">
-        <v>2.9564552482708652E-2</v>
+        <v>0.02956455248270865</v>
       </c>
       <c r="K30">
-        <v>8.9025223074148897E-5</v>
+        <v>8.90252230741489E-05</v>
       </c>
       <c r="L30">
-        <v>5.9216881344832328E-2</v>
+        <v>0.05921688134483233</v>
       </c>
       <c r="M30">
-        <v>-0.22377239468193871</v>
+        <v>-0.2237723946819387</v>
       </c>
       <c r="N30">
-        <v>-7.8354038824956451E-2</v>
+        <v>-0.07835403882495645</v>
       </c>
       <c r="O30">
-        <v>-0.80490277310972635</v>
+        <v>-0.8049027731097264</v>
       </c>
       <c r="P30">
-        <v>0.38254041293970742</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A31" s="2"/>
+        <v>0.3825404129397074</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16">
+      <c r="A31" s="1"/>
       <c r="B31" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C31">
-        <v>-0.63982974083758659</v>
+        <v>-0.6398297408375866</v>
       </c>
       <c r="D31">
-        <v>0.76851677964439724</v>
+        <v>0.7685167796443972</v>
       </c>
       <c r="E31">
-        <v>2.8548548343305991E-2</v>
+        <v>0.02854854834330599</v>
       </c>
       <c r="F31">
-        <v>0.22979068081907081</v>
+        <v>0.2297906808190708</v>
       </c>
       <c r="G31">
-        <v>3.0039134688561949E-2</v>
+        <v>0.03003913468856195</v>
       </c>
       <c r="H31">
-        <v>-7.8357894287930038E-2</v>
+        <v>-0.07835789428793004</v>
       </c>
       <c r="I31">
         <v>-1092.583836206036</v>
       </c>
       <c r="J31">
-        <v>5.5590265844699749E-4</v>
+        <v>0.0005559026584469975</v>
       </c>
       <c r="K31">
-        <v>5.7815428422945887E-4</v>
+        <v>0.0005781542842294589</v>
       </c>
       <c r="L31">
-        <v>7.8532201527685933E-2</v>
+        <v>0.07853220152768593</v>
       </c>
       <c r="M31">
-        <v>-0.16162848306625829</v>
+        <v>-0.1616284830662583</v>
       </c>
       <c r="N31">
-        <v>1.125176244882716E-2</v>
+        <v>0.01125176244882716</v>
       </c>
       <c r="O31">
-        <v>-1.736439040660301E-5</v>
+        <v>-1.736439040660301E-05</v>
       </c>
       <c r="P31">
-        <v>9.9964799009737496E-4</v>
+        <v>0.000999647990097375</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="A20:A23"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="A28:A31"/>
     <mergeCell ref="C1:I1"/>
     <mergeCell ref="J1:P1"/>
     <mergeCell ref="A4:A7"/>
     <mergeCell ref="A8:A11"/>
     <mergeCell ref="A12:A15"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="A28:A31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Finish results for starting value: 0.
</commit_message>
<xml_diff>
--- a/results/full_sample.xlsx
+++ b/results/full_sample.xlsx
@@ -538,34 +538,34 @@
         <v>21</v>
       </c>
       <c r="C4">
-        <v>0.7098381214420242</v>
+        <v>0.709838121424159</v>
       </c>
       <c r="D4">
-        <v>-0.7043648547885318</v>
+        <v>-0.7043648548065328</v>
       </c>
       <c r="E4">
-        <v>0.02251668933999882</v>
+        <v>0.02251668865119556</v>
       </c>
       <c r="F4">
-        <v>-0.1048481349071416</v>
+        <v>-0.1048481457669956</v>
       </c>
       <c r="G4">
-        <v>-15.68933939555135</v>
+        <v>-15.68933939568382</v>
       </c>
       <c r="J4">
-        <v>-1.008436364782866</v>
+        <v>-1.008436362205496</v>
       </c>
       <c r="K4">
-        <v>1.002846617733262</v>
+        <v>1.002846615199675</v>
       </c>
       <c r="L4">
-        <v>0.0008386423082800989</v>
+        <v>0.0008386433658731404</v>
       </c>
       <c r="M4">
-        <v>-0.07396385049726613</v>
+        <v>-0.07396382173572996</v>
       </c>
       <c r="N4">
-        <v>-0.02346185189357817</v>
+        <v>-0.02346185170250373</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -574,34 +574,34 @@
         <v>22</v>
       </c>
       <c r="C5">
-        <v>0.4951157913965695</v>
+        <v>0.4951174013371049</v>
       </c>
       <c r="D5">
-        <v>-0.868827000220375</v>
+        <v>-0.8688260828237517</v>
       </c>
       <c r="E5">
-        <v>0.07920885978259726</v>
+        <v>0.0792089098900229</v>
       </c>
       <c r="F5">
-        <v>0.05452386691006994</v>
+        <v>0.05452322129049693</v>
       </c>
       <c r="G5">
-        <v>-50.22228405238424</v>
+        <v>-50.22228417872717</v>
       </c>
       <c r="J5">
-        <v>-0.7864010003016408</v>
+        <v>-0.7864008077140071</v>
       </c>
       <c r="K5">
-        <v>0.69031491996577</v>
+        <v>0.6903147245254549</v>
       </c>
       <c r="L5">
-        <v>0.0668332998299893</v>
+        <v>0.06683330590921639</v>
       </c>
       <c r="M5">
-        <v>-0.2478746759656949</v>
+        <v>-0.2478746442946916</v>
       </c>
       <c r="N5">
-        <v>0.003686075776349947</v>
+        <v>0.003686079274810859</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -610,19 +610,19 @@
         <v>23</v>
       </c>
       <c r="C6">
-        <v>0.7154367184556623</v>
+        <v>0.7154367294421816</v>
       </c>
       <c r="D6">
-        <v>-0.6986775453711593</v>
+        <v>-0.6986775341180164</v>
       </c>
       <c r="E6">
-        <v>-0.2216961732569897</v>
+        <v>-0.2216962304415145</v>
       </c>
       <c r="F6">
-        <v>-0.7903494778953134</v>
+        <v>-0.7903510745430192</v>
       </c>
       <c r="G6">
-        <v>-2.565327611428497</v>
+        <v>-2.565327538908753</v>
       </c>
       <c r="J6">
         <v>-0.02635555574131339</v>
@@ -646,19 +646,19 @@
         <v>24</v>
       </c>
       <c r="C7">
-        <v>0.5741374456649357</v>
+        <v>0.5741374184962693</v>
       </c>
       <c r="D7">
-        <v>-0.8187589424738703</v>
+        <v>-0.8187589615275936</v>
       </c>
       <c r="E7">
-        <v>0.07926192535060521</v>
+        <v>0.07926191665981962</v>
       </c>
       <c r="F7">
-        <v>-0.07491298982348316</v>
+        <v>-0.07491292752311646</v>
       </c>
       <c r="G7">
-        <v>0.02250866737289285</v>
+        <v>0.02250867104918054</v>
       </c>
       <c r="J7">
         <v>0.2587221439061361</v>
@@ -684,19 +684,19 @@
         <v>21</v>
       </c>
       <c r="C8">
-        <v>-0.7044579395342766</v>
+        <v>-0.7044567187806103</v>
       </c>
       <c r="D8">
-        <v>0.7097457429751082</v>
+        <v>0.7097469514733179</v>
       </c>
       <c r="E8">
-        <v>0.1262528027031307</v>
+        <v>0.1262411707105019</v>
       </c>
       <c r="F8">
-        <v>-0.2430897441506744</v>
+        <v>-0.2431365207358937</v>
       </c>
       <c r="G8">
-        <v>7.850918115383918</v>
+        <v>7.850925357428166</v>
       </c>
       <c r="J8">
         <v>43.19112242833656</v>
@@ -720,34 +720,34 @@
         <v>22</v>
       </c>
       <c r="C9">
-        <v>-0.4950584662080166</v>
+        <v>-0.4950578647948832</v>
       </c>
       <c r="D9">
-        <v>0.8688597570740404</v>
+        <v>0.8688600997818102</v>
       </c>
       <c r="E9">
-        <v>0.07920441190513589</v>
+        <v>0.07920438220063698</v>
       </c>
       <c r="F9">
-        <v>0.05440953419999674</v>
+        <v>0.05440984276865816</v>
       </c>
       <c r="G9">
-        <v>45.50989231510833</v>
+        <v>45.50989226623803</v>
       </c>
       <c r="J9">
-        <v>0.789779583270067</v>
+        <v>0.7897800162999066</v>
       </c>
       <c r="K9">
-        <v>-0.6935217361869722</v>
+        <v>-0.6935221643312095</v>
       </c>
       <c r="L9">
-        <v>0.06669109430122834</v>
+        <v>0.06669108186216435</v>
       </c>
       <c r="M9">
-        <v>-0.2490975931274899</v>
+        <v>-0.2490977430243676</v>
       </c>
       <c r="N9">
-        <v>1.567155538521835</v>
+        <v>1.567155545411448</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -771,19 +771,19 @@
         <v>1.202325691000929</v>
       </c>
       <c r="J10">
-        <v>5.481174654556422</v>
+        <v>5.481173967358281</v>
       </c>
       <c r="K10">
-        <v>3.236681858681239</v>
+        <v>3.236682058183399</v>
       </c>
       <c r="L10">
-        <v>-1.072841594960227</v>
+        <v>-1.072841450705498</v>
       </c>
       <c r="M10">
-        <v>0.600354139001277</v>
+        <v>0.6003564245890757</v>
       </c>
       <c r="N10">
-        <v>-1.294523408058434</v>
+        <v>-1.294525327934617</v>
       </c>
     </row>
     <row r="11" spans="1:16">
@@ -792,34 +792,34 @@
         <v>24</v>
       </c>
       <c r="C11">
-        <v>0.7615809734138235</v>
+        <v>0.7615661890233265</v>
       </c>
       <c r="D11">
-        <v>-0.6480697665353834</v>
+        <v>-0.6480871390026202</v>
       </c>
       <c r="E11">
-        <v>0.06775331007101229</v>
+        <v>0.06776645399750968</v>
       </c>
       <c r="F11">
-        <v>-0.1375796395177813</v>
+        <v>-0.1375952508607388</v>
       </c>
       <c r="G11">
-        <v>1.543911226510316</v>
+        <v>1.54391159979668</v>
       </c>
       <c r="J11">
-        <v>-0.2537734547183552</v>
+        <v>-0.2537703572811663</v>
       </c>
       <c r="K11">
-        <v>0.4663503935333462</v>
+        <v>0.4663469400252133</v>
       </c>
       <c r="L11">
-        <v>0.07652194954252714</v>
+        <v>0.0765219550105843</v>
       </c>
       <c r="M11">
-        <v>-0.09017831898554039</v>
+        <v>-0.0901786962830054</v>
       </c>
       <c r="N11">
-        <v>1.547280156065749</v>
+        <v>1.547280150959703</v>
       </c>
     </row>
     <row r="12" spans="1:16">
@@ -830,40 +830,40 @@
         <v>21</v>
       </c>
       <c r="C12">
-        <v>0.9774859901853097</v>
+        <v>0.9774860038907432</v>
       </c>
       <c r="D12">
-        <v>0.2110003575999218</v>
+        <v>0.2110002944970373</v>
       </c>
       <c r="E12">
-        <v>-0.7504599496975273</v>
+        <v>-0.7504605364110853</v>
       </c>
       <c r="F12">
-        <v>0.7997881906877118</v>
+        <v>0.7997849466677615</v>
       </c>
       <c r="G12">
-        <v>2.079635739742439</v>
+        <v>2.079634326256628</v>
       </c>
       <c r="H12">
-        <v>-24.43232322829261</v>
+        <v>-24.43232456647322</v>
       </c>
       <c r="J12">
-        <v>-0.8878367720378068</v>
+        <v>-0.8878371774424391</v>
       </c>
       <c r="K12">
-        <v>0.882894253376026</v>
+        <v>0.8828946577927232</v>
       </c>
       <c r="L12">
-        <v>0.0008206426430817841</v>
+        <v>0.000820642913212596</v>
       </c>
       <c r="M12">
-        <v>-0.07599528089600012</v>
+        <v>-0.07599525702237536</v>
       </c>
       <c r="N12">
-        <v>-0.02356525631407446</v>
+        <v>-0.02356525107181082</v>
       </c>
       <c r="O12">
-        <v>1.136082901697407</v>
+        <v>1.136082408956695</v>
       </c>
     </row>
     <row r="13" spans="1:16">
@@ -872,22 +872,22 @@
         <v>22</v>
       </c>
       <c r="C13">
-        <v>0.7516053734108572</v>
+        <v>0.7516053174122794</v>
       </c>
       <c r="D13">
-        <v>-0.6596132743787885</v>
+        <v>-0.6596133396558523</v>
       </c>
       <c r="E13">
-        <v>0.06674291266235197</v>
+        <v>0.06674291432958364</v>
       </c>
       <c r="F13">
-        <v>-0.2482506625175557</v>
+        <v>-0.2482501801507858</v>
       </c>
       <c r="G13">
-        <v>0.003685920950879629</v>
+        <v>0.003685923931887904</v>
       </c>
       <c r="H13">
-        <v>-1.047832422885642</v>
+        <v>-1.047831593073773</v>
       </c>
       <c r="J13">
         <v>0.0002875790851084508</v>
@@ -914,40 +914,40 @@
         <v>23</v>
       </c>
       <c r="C14">
-        <v>0.9880942860639754</v>
+        <v>0.9880942860847126</v>
       </c>
       <c r="D14">
-        <v>0.1538495460290427</v>
+        <v>0.1538495458973727</v>
       </c>
       <c r="E14">
-        <v>0.06080773224107452</v>
+        <v>0.06080772441915611</v>
       </c>
       <c r="F14">
-        <v>-0.2203478743561139</v>
+        <v>-0.2203478628010135</v>
       </c>
       <c r="G14">
-        <v>3.22394628555047</v>
+        <v>3.223946284529929</v>
       </c>
       <c r="H14">
-        <v>0.02358347009745586</v>
+        <v>0.02358346987128835</v>
       </c>
       <c r="J14">
-        <v>0.03260096609175704</v>
+        <v>0.03260245534916581</v>
       </c>
       <c r="K14">
-        <v>2.398570545776159E-05</v>
+        <v>2.127956400327884E-05</v>
       </c>
       <c r="L14">
-        <v>0.05920939137027812</v>
+        <v>0.05921318600546775</v>
       </c>
       <c r="M14">
-        <v>-0.223982863030423</v>
+        <v>-0.223965678708776</v>
       </c>
       <c r="N14">
-        <v>-0.08309331636021043</v>
+        <v>-0.08308531615432913</v>
       </c>
       <c r="O14">
-        <v>-0.8089422252396085</v>
+        <v>-0.8088804624166962</v>
       </c>
     </row>
     <row r="15" spans="1:16">
@@ -956,22 +956,22 @@
         <v>24</v>
       </c>
       <c r="C15">
-        <v>0.7033050953208038</v>
+        <v>0.7033050888063973</v>
       </c>
       <c r="D15">
-        <v>0.7108885644611309</v>
+        <v>0.7108885709161049</v>
       </c>
       <c r="E15">
-        <v>0.07375442281381046</v>
+        <v>0.07375441594451834</v>
       </c>
       <c r="F15">
-        <v>-0.1054358592556594</v>
+        <v>-0.1054360420123764</v>
       </c>
       <c r="G15">
-        <v>0.02475336491081646</v>
+        <v>0.02475336635879038</v>
       </c>
       <c r="H15">
-        <v>-0.1271351954521083</v>
+        <v>-0.1271352062475561</v>
       </c>
       <c r="J15">
         <v>0.0005564141499510517</v>
@@ -1000,40 +1000,40 @@
         <v>21</v>
       </c>
       <c r="C16">
-        <v>-0.7090718105932952</v>
+        <v>-0.7090749030746691</v>
       </c>
       <c r="D16">
-        <v>0.7051362855134072</v>
+        <v>0.7051331686116852</v>
       </c>
       <c r="E16">
-        <v>0.0008310745674540872</v>
+        <v>0.0008454985959567293</v>
       </c>
       <c r="F16">
-        <v>-0.07603845716546016</v>
+        <v>-0.07609126113049207</v>
       </c>
       <c r="G16">
-        <v>-1.594270224042217</v>
+        <v>-1.594326038658507</v>
       </c>
       <c r="H16">
-        <v>1.422661328159769</v>
+        <v>1.422240593000021</v>
       </c>
       <c r="J16">
-        <v>-380.693533592581</v>
+        <v>-380.9848901678577</v>
       </c>
       <c r="K16">
-        <v>378.6153372479027</v>
+        <v>378.9142337246403</v>
       </c>
       <c r="L16">
-        <v>0.0009199976451660269</v>
+        <v>0.0009084156548920764</v>
       </c>
       <c r="M16">
-        <v>-0.07584713680197112</v>
+        <v>-0.07591156862764555</v>
       </c>
       <c r="N16">
-        <v>1.593964232857632</v>
+        <v>1.59387768663573</v>
       </c>
       <c r="O16">
-        <v>-0.00264917575231065</v>
+        <v>-0.002646912214969954</v>
       </c>
     </row>
     <row r="17" spans="1:16">
@@ -1042,40 +1042,40 @@
         <v>22</v>
       </c>
       <c r="C17">
-        <v>0.7516508672646135</v>
+        <v>0.7516505208070711</v>
       </c>
       <c r="D17">
-        <v>-0.6595613757656622</v>
+        <v>-0.6595617685997213</v>
       </c>
       <c r="E17">
-        <v>0.06676215683422725</v>
+        <v>0.06676183667599031</v>
       </c>
       <c r="F17">
-        <v>-0.2488023979690625</v>
+        <v>-0.2488013281547434</v>
       </c>
       <c r="G17">
-        <v>1.567108760181873</v>
+        <v>1.567108715126415</v>
       </c>
       <c r="H17">
-        <v>1.048802788796408</v>
+        <v>1.048794957372736</v>
       </c>
       <c r="J17">
-        <v>-2.502611679192388</v>
+        <v>-2.502599357115216</v>
       </c>
       <c r="K17">
-        <v>2.194267637502465</v>
+        <v>2.194255690912645</v>
       </c>
       <c r="L17">
-        <v>0.06669510370130183</v>
+        <v>0.06669520612804566</v>
       </c>
       <c r="M17">
-        <v>-0.2498806588699114</v>
+        <v>-0.2498797157698865</v>
       </c>
       <c r="N17">
-        <v>1.567050667144039</v>
+        <v>1.567050643247503</v>
       </c>
       <c r="O17">
-        <v>-0.314588346489649</v>
+        <v>-0.3145896719217678</v>
       </c>
     </row>
     <row r="18" spans="1:16">
@@ -1084,40 +1084,40 @@
         <v>23</v>
       </c>
       <c r="C18">
-        <v>-0.04782147420343646</v>
+        <v>-0.04541780833798722</v>
       </c>
       <c r="D18">
-        <v>-0.9988558994359621</v>
+        <v>-0.9989682584138067</v>
       </c>
       <c r="E18">
-        <v>0.07588179273400497</v>
+        <v>0.07565941105184355</v>
       </c>
       <c r="F18">
-        <v>-0.1897320256817751</v>
+        <v>-0.1908466566018453</v>
       </c>
       <c r="G18">
-        <v>-1.613683767079483</v>
+        <v>-1.613383092264097</v>
       </c>
       <c r="H18">
-        <v>0.0179913248708101</v>
+        <v>0.01794490614628489</v>
       </c>
       <c r="J18">
-        <v>1.610638011049659</v>
+        <v>1.610638435140205</v>
       </c>
       <c r="K18">
-        <v>0.003877913977938663</v>
+        <v>0.003877560919212601</v>
       </c>
       <c r="L18">
-        <v>0.05867533449522708</v>
+        <v>0.05867533818450962</v>
       </c>
       <c r="M18">
-        <v>-0.2236385302136577</v>
+        <v>-0.2236385236731886</v>
       </c>
       <c r="N18">
-        <v>1.65419121399958</v>
+        <v>1.654191206751706</v>
       </c>
       <c r="O18">
-        <v>0.01640883315131444</v>
+        <v>0.01640883014325819</v>
       </c>
     </row>
     <row r="19" spans="1:16">
@@ -1126,40 +1126,40 @@
         <v>24</v>
       </c>
       <c r="C19">
-        <v>0.7578408481315352</v>
+        <v>0.7578409545179549</v>
       </c>
       <c r="D19">
-        <v>0.6524395023687195</v>
+        <v>0.6524393788035275</v>
       </c>
       <c r="E19">
-        <v>0.07388717905487292</v>
+        <v>0.07388718327957092</v>
       </c>
       <c r="F19">
-        <v>-0.1070431088417302</v>
+        <v>-0.1070429185261272</v>
       </c>
       <c r="G19">
-        <v>1.5461189536237</v>
+        <v>1.546118945238499</v>
       </c>
       <c r="H19">
-        <v>0.1263654353812654</v>
+        <v>0.126365514847335</v>
       </c>
       <c r="J19">
-        <v>0.2694238593883589</v>
+        <v>0.2694245874272864</v>
       </c>
       <c r="K19">
-        <v>0.3232431072770122</v>
+        <v>0.3232423478894169</v>
       </c>
       <c r="L19">
-        <v>0.07354144521613745</v>
+        <v>0.07354145837067667</v>
       </c>
       <c r="M19">
-        <v>-0.1055496786318387</v>
+        <v>-0.1055495801041808</v>
       </c>
       <c r="N19">
-        <v>1.546091199902045</v>
+        <v>1.546091192454078</v>
       </c>
       <c r="O19">
-        <v>0.3053415399855133</v>
+        <v>0.3053416392146496</v>
       </c>
     </row>
     <row r="20" spans="1:16">
@@ -1254,22 +1254,22 @@
         <v>23</v>
       </c>
       <c r="C22">
-        <v>0.7000936373097983</v>
+        <v>0.7000936373123587</v>
       </c>
       <c r="D22">
-        <v>0.714051047893883</v>
+        <v>0.7140510478913726</v>
       </c>
       <c r="E22">
-        <v>0.1021026990491623</v>
+        <v>0.1021027043340019</v>
       </c>
       <c r="F22">
-        <v>-0.1892459790940466</v>
+        <v>-0.1892458303693788</v>
       </c>
       <c r="G22">
-        <v>4.725730188048101</v>
+        <v>4.725730185531894</v>
       </c>
       <c r="H22">
-        <v>3.478380491093048</v>
+        <v>3.478380489162676</v>
       </c>
       <c r="J22">
         <v>0.0009958101240693897</v>
@@ -1296,22 +1296,22 @@
         <v>24</v>
       </c>
       <c r="C23">
-        <v>0.7071098409300589</v>
+        <v>0.7071098409300689</v>
       </c>
       <c r="D23">
-        <v>0.7071037214298825</v>
+        <v>0.7071037214298725</v>
       </c>
       <c r="E23">
-        <v>0.07852964963935608</v>
+        <v>0.07852964957127639</v>
       </c>
       <c r="F23">
-        <v>-0.1616363980561757</v>
+        <v>-0.1616363979732369</v>
       </c>
       <c r="G23">
-        <v>0.01125629529699257</v>
+        <v>0.01125629533192462</v>
       </c>
       <c r="H23">
-        <v>0.01725818088176704</v>
+        <v>0.01725818096435809</v>
       </c>
       <c r="J23">
         <v>0.001000000000000008</v>
@@ -1358,22 +1358,22 @@
         <v>-8.342989800165364</v>
       </c>
       <c r="J24">
-        <v>-0.0001485025403608644</v>
+        <v>-0.0001485196493705326</v>
       </c>
       <c r="K24">
-        <v>1.381400503901313E-05</v>
+        <v>1.381400287788994E-05</v>
       </c>
       <c r="L24">
-        <v>0.1020167588733892</v>
+        <v>0.1020167588643707</v>
       </c>
       <c r="M24">
-        <v>-0.1892600264667267</v>
+        <v>-0.1892600273497442</v>
       </c>
       <c r="N24">
-        <v>0.0007076745992829673</v>
+        <v>0.0007076745986418191</v>
       </c>
       <c r="O24">
-        <v>-0.0003621240646972985</v>
+        <v>-0.0003621411749867451</v>
       </c>
     </row>
     <row r="25" spans="1:16">
@@ -1382,22 +1382,22 @@
         <v>22</v>
       </c>
       <c r="C25">
-        <v>-0.7315403412724705</v>
+        <v>-0.7315259168507862</v>
       </c>
       <c r="D25">
-        <v>0.6817981596477792</v>
+        <v>0.6818136877577514</v>
       </c>
       <c r="E25">
-        <v>0.06796006736228839</v>
+        <v>0.06796370088910662</v>
       </c>
       <c r="F25">
-        <v>-0.225293720824576</v>
+        <v>-0.2253312913318439</v>
       </c>
       <c r="G25">
-        <v>-0.02016345811127186</v>
+        <v>-0.02016292546854981</v>
       </c>
       <c r="H25">
-        <v>-12.94219533959819</v>
+        <v>-12.93796713673039</v>
       </c>
       <c r="J25">
         <v>0.001001971637650307</v>
@@ -1466,22 +1466,22 @@
         <v>24</v>
       </c>
       <c r="C27">
-        <v>-0.9182280452066156</v>
+        <v>-0.9105388727003462</v>
       </c>
       <c r="D27">
-        <v>0.396052118713613</v>
+        <v>0.4134234698939865</v>
       </c>
       <c r="E27">
-        <v>0.07197119059425357</v>
+        <v>0.07182844798550909</v>
       </c>
       <c r="F27">
-        <v>-0.1086570392507689</v>
+        <v>-0.108872348717634</v>
       </c>
       <c r="G27">
-        <v>-0.108563304215763</v>
+        <v>-0.1035193405593236</v>
       </c>
       <c r="H27">
-        <v>-2.684786587616844</v>
+        <v>-2.98058526336463</v>
       </c>
       <c r="J27">
         <v>0.001005200338459678</v>
@@ -1510,46 +1510,46 @@
         <v>21</v>
       </c>
       <c r="C28">
-        <v>-0.1704167433910599</v>
+        <v>-0.1704167405842537</v>
       </c>
       <c r="D28">
-        <v>0.9853720790605308</v>
+        <v>0.9853720795457011</v>
       </c>
       <c r="E28">
-        <v>0.09435244370539617</v>
+        <v>0.09435243202051799</v>
       </c>
       <c r="F28">
-        <v>-0.09986669010508539</v>
+        <v>-0.09986668875507175</v>
       </c>
       <c r="G28">
-        <v>0.08907253530897012</v>
+        <v>0.08907233567849963</v>
       </c>
       <c r="H28">
-        <v>0.02358984580584816</v>
+        <v>0.02358971182780927</v>
       </c>
       <c r="I28">
-        <v>-0.001104977870285756</v>
+        <v>-0.001105000015157252</v>
       </c>
       <c r="J28">
-        <v>-0.8791879668761952</v>
+        <v>-0.8791880709594413</v>
       </c>
       <c r="K28">
-        <v>0.8743519750411963</v>
+        <v>0.8743520840195337</v>
       </c>
       <c r="L28">
-        <v>0.0005417878866458317</v>
+        <v>0.0005417905300352542</v>
       </c>
       <c r="M28">
-        <v>-0.07645911373322599</v>
+        <v>-0.0764591037305877</v>
       </c>
       <c r="N28">
-        <v>-0.02313861396580737</v>
+        <v>-0.02313859286838172</v>
       </c>
       <c r="O28">
-        <v>1.141644745624486</v>
+        <v>1.141644621649656</v>
       </c>
       <c r="P28">
-        <v>-0.0007414576441306117</v>
+        <v>-0.0007415277058695335</v>
       </c>
     </row>
     <row r="29" spans="1:16">
@@ -1558,25 +1558,25 @@
         <v>22</v>
       </c>
       <c r="C29">
-        <v>0.7531422248115809</v>
+        <v>0.7531460506550851</v>
       </c>
       <c r="D29">
-        <v>-0.6578579028212793</v>
+        <v>-0.6578535413509916</v>
       </c>
       <c r="E29">
-        <v>0.06666808365576414</v>
+        <v>0.06666755875355909</v>
       </c>
       <c r="F29">
-        <v>-0.2491696081654818</v>
+        <v>-0.2491756862722024</v>
       </c>
       <c r="G29">
-        <v>0.004123915982426355</v>
+        <v>0.004124049604997121</v>
       </c>
       <c r="H29">
-        <v>-1.07555160128354</v>
+        <v>-1.07555274140744</v>
       </c>
       <c r="I29">
-        <v>-2.620643412994134</v>
+        <v>-2.620523819797156</v>
       </c>
       <c r="J29">
         <v>0.0002872417743139459</v>
@@ -1606,46 +1606,46 @@
         <v>23</v>
       </c>
       <c r="C30">
-        <v>-0.05395292895101558</v>
+        <v>-0.05395292895189671</v>
       </c>
       <c r="D30">
-        <v>0.998543480006357</v>
+        <v>0.9985434800063084</v>
       </c>
       <c r="E30">
-        <v>0.05105829561359689</v>
+        <v>0.05105830091872841</v>
       </c>
       <c r="F30">
-        <v>-0.1954875763377007</v>
+        <v>-0.1954875353090587</v>
       </c>
       <c r="G30">
-        <v>-0.1877447483871651</v>
+        <v>-0.1877447440663715</v>
       </c>
       <c r="H30">
-        <v>-0.12862202168276</v>
+        <v>-0.1286220179767376</v>
       </c>
       <c r="I30">
-        <v>-0.01966590661180215</v>
+        <v>-0.01966590587380392</v>
       </c>
       <c r="J30">
-        <v>0.02956455248270865</v>
+        <v>0.02956458681318301</v>
       </c>
       <c r="K30">
-        <v>8.90252230741489E-05</v>
+        <v>8.898982777003431E-05</v>
       </c>
       <c r="L30">
-        <v>0.05921688134483233</v>
+        <v>0.05921688485624587</v>
       </c>
       <c r="M30">
-        <v>-0.2237723946819387</v>
+        <v>-0.2237725396091237</v>
       </c>
       <c r="N30">
-        <v>-0.07835403882495645</v>
+        <v>-0.07835397738370777</v>
       </c>
       <c r="O30">
-        <v>-0.8049027731097264</v>
+        <v>-0.8049020769029773</v>
       </c>
       <c r="P30">
-        <v>0.3825404129397074</v>
+        <v>0.3825401462632464</v>
       </c>
     </row>
     <row r="31" spans="1:16">
@@ -1654,46 +1654,46 @@
         <v>24</v>
       </c>
       <c r="C31">
-        <v>-0.6398297408375866</v>
+        <v>-0.6399409290937439</v>
       </c>
       <c r="D31">
-        <v>0.7685167796443972</v>
+        <v>0.7684241074777763</v>
       </c>
       <c r="E31">
-        <v>0.02854854834330599</v>
+        <v>0.02854685782067485</v>
       </c>
       <c r="F31">
-        <v>0.2297906808190708</v>
+        <v>0.2297228834772579</v>
       </c>
       <c r="G31">
-        <v>0.03003913468856195</v>
+        <v>0.03002158436976246</v>
       </c>
       <c r="H31">
-        <v>-0.07835789428793004</v>
+        <v>-0.1311001623395306</v>
       </c>
       <c r="I31">
-        <v>-1092.583836206036</v>
+        <v>-1093.146085553029</v>
       </c>
       <c r="J31">
-        <v>0.0005559026584469975</v>
+        <v>0.0005559026595429201</v>
       </c>
       <c r="K31">
-        <v>0.0005781542842294589</v>
+        <v>0.0005781542851671488</v>
       </c>
       <c r="L31">
-        <v>0.07853220152768593</v>
+        <v>0.07853220704964289</v>
       </c>
       <c r="M31">
-        <v>-0.1616284830662583</v>
+        <v>-0.1616284827868015</v>
       </c>
       <c r="N31">
-        <v>0.01125176244882716</v>
+        <v>0.01125176237556763</v>
       </c>
       <c r="O31">
-        <v>-1.736439040660301E-05</v>
+        <v>-1.736438764454146E-05</v>
       </c>
       <c r="P31">
-        <v>0.000999647990097375</v>
+        <v>0.0009996479900988332</v>
       </c>
     </row>
     <row r="32" spans="1:16">
@@ -1704,40 +1704,40 @@
         <v>21</v>
       </c>
       <c r="C32">
-        <v>0.9941876672688381</v>
+        <v>0.994187667068993</v>
       </c>
       <c r="D32">
-        <v>0.1076611521111814</v>
+        <v>0.1076611539406717</v>
       </c>
       <c r="E32">
-        <v>0.06243114902311073</v>
+        <v>0.06243112669240598</v>
       </c>
       <c r="F32">
-        <v>-0.214212169959094</v>
+        <v>-0.2142122347735561</v>
       </c>
       <c r="G32">
-        <v>-0.06752723252906526</v>
+        <v>-0.06752724724328267</v>
       </c>
       <c r="H32">
-        <v>-0.02001023281851924</v>
+        <v>-0.02001023668062291</v>
       </c>
       <c r="J32">
-        <v>-0.7592545198792477</v>
+        <v>-0.7592748373184847</v>
       </c>
       <c r="K32">
-        <v>0.7550530123375351</v>
+        <v>0.7550716968140087</v>
       </c>
       <c r="L32">
-        <v>0.000533951932499174</v>
+        <v>0.0005295381186969019</v>
       </c>
       <c r="M32">
-        <v>-0.07599871989917226</v>
+        <v>-0.07600710405390634</v>
       </c>
       <c r="N32">
-        <v>-0.02325240528949909</v>
+        <v>-0.02326626212531237</v>
       </c>
       <c r="O32">
-        <v>1.322233280946119</v>
+        <v>1.322177650832585</v>
       </c>
     </row>
     <row r="33" spans="1:15">
@@ -1746,22 +1746,22 @@
         <v>22</v>
       </c>
       <c r="C33">
-        <v>0.7516348697488138</v>
+        <v>0.7516356472842874</v>
       </c>
       <c r="D33">
-        <v>-0.6595794975758583</v>
+        <v>-0.6595786126886428</v>
       </c>
       <c r="E33">
-        <v>0.06670762555186247</v>
+        <v>0.06670817977653899</v>
       </c>
       <c r="F33">
-        <v>-0.2483575762308422</v>
+        <v>-0.2483572814097438</v>
       </c>
       <c r="G33">
-        <v>0.003695374085139963</v>
+        <v>0.003695481821577288</v>
       </c>
       <c r="H33">
-        <v>-1.047382512883674</v>
+        <v>-1.047375987935854</v>
       </c>
       <c r="J33">
         <v>0.000287635776838243</v>
@@ -1788,40 +1788,40 @@
         <v>23</v>
       </c>
       <c r="C34">
-        <v>0.9926423773030885</v>
+        <v>0.9926423774005686</v>
       </c>
       <c r="D34">
-        <v>0.1210830738912044</v>
+        <v>0.1210830730920692</v>
       </c>
       <c r="E34">
-        <v>0.06045923553741416</v>
+        <v>0.06045923614224346</v>
       </c>
       <c r="F34">
-        <v>-0.2221195310801078</v>
+        <v>-0.2221193797542841</v>
       </c>
       <c r="G34">
-        <v>-0.08246947428431807</v>
+        <v>-0.08246946870803593</v>
       </c>
       <c r="H34">
-        <v>-0.02407687258934132</v>
+        <v>-0.02407687121513873</v>
       </c>
       <c r="J34">
-        <v>0.02726048875290267</v>
+        <v>0.02726112220237813</v>
       </c>
       <c r="K34">
-        <v>0.0001779829308553644</v>
+        <v>0.0001776680990342017</v>
       </c>
       <c r="L34">
-        <v>0.05898636222537064</v>
+        <v>0.05898655754058675</v>
       </c>
       <c r="M34">
-        <v>-0.2239159852131893</v>
+        <v>-0.2239167652587719</v>
       </c>
       <c r="N34">
-        <v>-0.08343165173602035</v>
+        <v>-0.08342983042415342</v>
       </c>
       <c r="O34">
-        <v>-0.9663201860981097</v>
+        <v>-0.9662895120170831</v>
       </c>
     </row>
     <row r="35" spans="1:15">
@@ -1830,22 +1830,22 @@
         <v>24</v>
       </c>
       <c r="C35">
-        <v>0.7008243932976027</v>
+        <v>0.7008243332110968</v>
       </c>
       <c r="D35">
-        <v>0.7133340566802808</v>
+        <v>0.7133341157866682</v>
       </c>
       <c r="E35">
-        <v>0.07353716227086454</v>
+        <v>0.0735371656838327</v>
       </c>
       <c r="F35">
-        <v>-0.1066706664519764</v>
+        <v>-0.1066707909404621</v>
       </c>
       <c r="G35">
-        <v>0.02467783435274407</v>
+        <v>0.02467783536997837</v>
       </c>
       <c r="H35">
-        <v>-0.1268919963534691</v>
+        <v>-0.1268920052844351</v>
       </c>
       <c r="J35">
         <v>0.0005562696162124333</v>

</xml_diff>